<commit_message>
add upload essay quiz
</commit_message>
<xml_diff>
--- a/src/main/resources/quiz_template.xlsx
+++ b/src/main/resources/quiz_template.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Kafila Projects\arabic-club-backend\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Kafila Projects\arabic-club-front-end\public\resources\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MULTIPLE_CHOICE" sheetId="1" r:id="rId1"/>
+    <sheet name="ESSAY" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
   <si>
     <t>number</t>
   </si>
@@ -114,6 +115,63 @@
   </si>
   <si>
     <t>Quiz Title AAAAA</t>
+  </si>
+  <si>
+    <t>MULTIPLE_CHOICE</t>
+  </si>
+  <si>
+    <t>ESSAY</t>
+  </si>
+  <si>
+    <t>ANSWER ESSAY</t>
+  </si>
+  <si>
+    <t>Answer essay 1</t>
+  </si>
+  <si>
+    <t>Answer essay 2</t>
+  </si>
+  <si>
+    <t>Answer essay 3</t>
+  </si>
+  <si>
+    <t>Answer essay 4</t>
+  </si>
+  <si>
+    <t>Answer essay 5</t>
+  </si>
+  <si>
+    <t>Answer essay 6</t>
+  </si>
+  <si>
+    <t>Answer essay 7</t>
+  </si>
+  <si>
+    <t>Answer essay 8</t>
+  </si>
+  <si>
+    <t>question essay 1</t>
+  </si>
+  <si>
+    <t>question essay 2</t>
+  </si>
+  <si>
+    <t>question essay 3</t>
+  </si>
+  <si>
+    <t>question essay 4</t>
+  </si>
+  <si>
+    <t>question essay 5</t>
+  </si>
+  <si>
+    <t>question essay 6</t>
+  </si>
+  <si>
+    <t>question essay 7</t>
+  </si>
+  <si>
+    <t>question essay 8</t>
   </si>
 </sst>
 </file>
@@ -191,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -226,6 +284,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -512,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="A1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +613,9 @@
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -598,31 +661,31 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="7" t="s">
         <v>11</v>
       </c>
@@ -890,4 +953,176 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
+        <v>50</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>3</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>7</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>8</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>